<commit_message>
P1 bug fixes for UI, Security.
</commit_message>
<xml_diff>
--- a/MyNPO/MyNPO/Documents/MyNPO_Bugs.xlsx
+++ b/MyNPO/MyNPO/Documents/MyNPO_Bugs.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\v-manipa\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\v-manipa\Source\Repos\quadrant\MyNPO\MyNPO\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{723F3B11-ABC4-4528-A369-4A226C20A871}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E3DBDB0-0D12-4147-80BE-FDE17B7FF605}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17490" windowHeight="7620" xr2:uid="{E764FEA4-55E6-47A7-B5D4-F95EB5C20911}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$3:$E$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$3:$G$3</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="57">
   <si>
     <t>BugID</t>
   </si>
@@ -162,6 +162,71 @@
   </si>
   <si>
     <t>MyNPO Bug List</t>
+  </si>
+  <si>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Fixed</t>
+  </si>
+  <si>
+    <t>Mani Parnandi</t>
+  </si>
+  <si>
+    <t>Not Started</t>
+  </si>
+  <si>
+    <t>Removed the SaiBaba menu.</t>
+  </si>
+  <si>
+    <t>Removed the Help menu. We don't About menu as this is internal app.
+Renamed the Contact to "Contact us".</t>
+  </si>
+  <si>
+    <t>Space is present in the drop down items which is good.</t>
+  </si>
+  <si>
+    <t>Desgin</t>
+  </si>
+  <si>
+    <t>Room Booking need to be re-designed</t>
+  </si>
+  <si>
+    <t>Senbaga</t>
+  </si>
+  <si>
+    <t>The Login page is designed simple for just user authentication only.
+This is internal application for admin users for temple operations</t>
+  </si>
+  <si>
+    <t>Design</t>
+  </si>
+  <si>
+    <t>Logout button/link is not present in the application</t>
+  </si>
+  <si>
+    <t>Fixed. Added a Logout link, upon clicking re-direct to Login page.</t>
+  </si>
+  <si>
+    <t>Need to add flyers from original site</t>
+  </si>
+  <si>
+    <t>Removed this menu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fixed. </t>
+  </si>
+  <si>
+    <t>Home page can be changed to latest flyer if possible or a picture.</t>
+  </si>
+  <si>
+    <t>Abhishekam Registration should be renamed as "Priest Services"</t>
+  </si>
+  <si>
+    <t>Priest services should have a calendar to know the bookings made and should also allow for registering the pooja events at temple and personal address</t>
   </si>
 </sst>
 </file>
@@ -192,7 +257,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -202,6 +267,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -230,6 +301,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -240,38 +320,34 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -588,38 +664,44 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{663B2713-C9A7-4F11-B015-FF990BD785C6}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:E33"/>
+  <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="81.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" customWidth="1"/>
-    <col min="4" max="4" width="17.7109375" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" customWidth="1"/>
+    <col min="4" max="4" width="64.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" customWidth="1"/>
+    <col min="7" max="7" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="8"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="9"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -627,355 +709,565 @@
         <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1</v>
+        <v>36</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>1</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
+      <c r="C4" s="2">
+        <v>4</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>54</v>
+      </c>
       <c r="E4" s="2"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4" s="2"/>
+      <c r="G4" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>2</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C5" s="2">
+        <v>1</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>3</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C6" s="2">
+        <v>1</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>4</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C7" s="2">
+        <v>4</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>5</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C8" s="2">
+        <v>3</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+    </row>
+    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>6</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-    </row>
-    <row r="10" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="C9" s="2">
+        <v>4</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>7</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
+      <c r="C10" s="3">
+        <v>1</v>
+      </c>
+      <c r="D10" s="3"/>
       <c r="E10" s="2"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>8</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
+      <c r="C11" s="2">
+        <v>3</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>51</v>
+      </c>
       <c r="E11" s="2"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>9</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="2"/>
+      <c r="C12" s="2">
+        <v>2</v>
+      </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>10</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="2"/>
+      <c r="C13" s="2">
+        <v>1</v>
+      </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
-    </row>
-    <row r="14" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+    </row>
+    <row r="14" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>11</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
+      <c r="C14" s="3">
+        <v>2</v>
+      </c>
+      <c r="D14" s="3"/>
       <c r="E14" s="2"/>
-    </row>
-    <row r="15" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+    </row>
+    <row r="15" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>12</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
+      <c r="C15" s="3">
+        <v>1</v>
+      </c>
+      <c r="D15" s="3"/>
       <c r="E15" s="2"/>
-    </row>
-    <row r="16" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+    </row>
+    <row r="16" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>13</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
       <c r="E16" s="2"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>14</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
+      <c r="C17" s="3">
+        <v>1</v>
+      </c>
+      <c r="D17" s="3"/>
       <c r="E17" s="2"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>15</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
+      <c r="C18" s="3">
+        <v>1</v>
+      </c>
+      <c r="D18" s="3"/>
       <c r="E18" s="2"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>16</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
+      <c r="C19" s="3">
+        <v>1</v>
+      </c>
+      <c r="D19" s="3"/>
       <c r="E19" s="2"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>17</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
+      <c r="C20" s="3">
+        <v>1</v>
+      </c>
+      <c r="D20" s="3"/>
       <c r="E20" s="2"/>
-    </row>
-    <row r="21" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+    </row>
+    <row r="21" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>18</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
+      <c r="C21" s="3">
+        <v>1</v>
+      </c>
+      <c r="D21" s="3"/>
       <c r="E21" s="2"/>
-    </row>
-    <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+    </row>
+    <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>19</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-    </row>
-    <row r="23" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="C22" s="3">
+        <v>1</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G22" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>20</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-    </row>
-    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="4">
+      <c r="C23" s="3">
+        <v>1</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G23" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="7">
         <v>21</v>
       </c>
-      <c r="B24" s="6" t="s">
+      <c r="B24" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
       <c r="E24" s="2"/>
-    </row>
-    <row r="25" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A25" s="4">
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+    </row>
+    <row r="25" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A25" s="7">
         <v>22</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="B25" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
       <c r="E25" s="2"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="4">
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="7">
         <v>23</v>
       </c>
-      <c r="B26" s="6" t="s">
+      <c r="B26" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
       <c r="E26" s="2"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="4">
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="7">
         <v>24</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="B27" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
       <c r="E27" s="2"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="4">
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="7">
         <v>25</v>
       </c>
-      <c r="B28" s="6" t="s">
+      <c r="B28" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
       <c r="E28" s="2"/>
-    </row>
-    <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="4">
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+    </row>
+    <row r="29" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="7">
         <v>26</v>
       </c>
-      <c r="B29" s="6" t="s">
+      <c r="B29" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
       <c r="E29" s="2"/>
-    </row>
-    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="4">
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+    </row>
+    <row r="30" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="7">
         <v>27</v>
       </c>
-      <c r="B30" s="6" t="s">
+      <c r="B30" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
       <c r="E30" s="2"/>
-    </row>
-    <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="4">
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+    </row>
+    <row r="31" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="7">
         <v>28</v>
       </c>
-      <c r="B31" s="6" t="s">
+      <c r="B31" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
       <c r="E31" s="2"/>
-    </row>
-    <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="4">
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+    </row>
+    <row r="32" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="7">
         <v>29</v>
       </c>
-      <c r="B32" s="6" t="s">
+      <c r="B32" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="4"/>
       <c r="E32" s="2"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="4">
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="7">
         <v>30</v>
       </c>
-      <c r="B33" s="5" t="s">
+      <c r="B33" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
+      <c r="C33" s="4"/>
+      <c r="D33" s="4"/>
       <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="7">
+        <v>31</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C34" s="2">
+        <v>1</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G34" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="10">
+        <v>32</v>
+      </c>
+      <c r="B35" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="C35">
+        <v>1</v>
+      </c>
+      <c r="E35" t="s">
+        <v>39</v>
+      </c>
+      <c r="F35" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A36" s="10">
+        <v>33</v>
+      </c>
+      <c r="B36" s="11" t="s">
+        <v>56</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A3:E3" xr:uid="{78C1B607-E0D5-48F6-804E-D8F0C2DBF031}">
-    <filterColumn colId="4">
+  <autoFilter ref="A3:G3" xr:uid="{78C1B607-E0D5-48F6-804E-D8F0C2DBF031}">
+    <filterColumn colId="6">
       <filters>
         <filter val="Status"/>
       </filters>
     </filterColumn>
   </autoFilter>
   <mergeCells count="1">
-    <mergeCell ref="A1:E2"/>
+    <mergeCell ref="A1:G2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>